<commit_message>
Initial commit node results component
</commit_message>
<xml_diff>
--- a/Components_Icons_Overview.xlsx
+++ b/Components_Icons_Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristjan.Nielsen\source\repos\GhSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F8EB25-7170-49C1-AF5B-71B4742CEC89}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D062C2B-1399-4695-96AB-C69040F72877}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="2685" windowWidth="25260" windowHeight="16980" xr2:uid="{BD94AA30-14AC-4672-A485-2DCD59B07C88}"/>
   </bookViews>
@@ -2402,7 +2402,7 @@
   <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Debugged colouring, results output and legend
</commit_message>
<xml_diff>
--- a/Components_Icons_Overview.xlsx
+++ b/Components_Icons_Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristjan.Nielsen\source\repos\GhSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D062C2B-1399-4695-96AB-C69040F72877}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B5447B-12B7-4DA2-9172-2D5818288691}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="2685" windowWidth="25260" windowHeight="16980" xr2:uid="{BD94AA30-14AC-4672-A485-2DCD59B07C88}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="149">
   <si>
     <t>GSA-Grasshopper Icons set</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Save</t>
   </si>
   <si>
-    <t>(hierachy)</t>
-  </si>
-  <si>
     <t>Component</t>
   </si>
   <si>
@@ -453,9 +450,6 @@
     <t>Grid Plane Surface Object holding both a grid plane and surface</t>
   </si>
   <si>
-    <t>GPS</t>
-  </si>
-  <si>
     <t>Node*</t>
   </si>
   <si>
@@ -481,6 +475,12 @@
   </si>
   <si>
     <t>Create a new Member 2D in Design layer (Brep/Surface)</t>
+  </si>
+  <si>
+    <t>Section*</t>
+  </si>
+  <si>
+    <t>(hierarchy)</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -623,6 +623,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -867,7 +873,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -890,108 +896,120 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1001,17 +1019,11 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2091,6 +2103,666 @@
         <a:xfrm>
           <a:off x="6886575" y="5029200"/>
           <a:ext cx="209524" cy="238095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>58616</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>21981</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>325283</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>326743</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4298F034-3057-41EF-AB62-45C050177E62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858001" y="5341327"/>
+          <a:ext cx="266667" cy="304762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>58616</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>36635</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>325283</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>293778</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D819E564-8EFB-48AB-9BE7-68E6098EE919}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858001" y="3831981"/>
+          <a:ext cx="266667" cy="257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>21981</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>21981</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>279124</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>307695</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33974CA6-7CF8-4ACE-A515-F60B94E0883A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6821366" y="13342327"/>
+          <a:ext cx="257143" cy="285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>21981</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>21981</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>279124</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>317219</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F09BD9DF-1363-483E-84C3-F4D4BAB90812}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6821366" y="12199327"/>
+          <a:ext cx="257143" cy="295238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>21981</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>21981</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>279124</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>317219</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A83AEB4-CD74-4D50-87F9-EA5D93DE6175}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6821366" y="12580327"/>
+          <a:ext cx="257143" cy="295238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>21981</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>21981</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>307695</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>326743</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0C504AF-4489-4EC5-8923-1628A9882E1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6821366" y="12961327"/>
+          <a:ext cx="285714" cy="304762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>58615</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>58616</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>258615</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>249092</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DCB95C5-69D3-4C0B-B358-C3A833656FF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858000" y="14902962"/>
+          <a:ext cx="200000" cy="190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>43962</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>21981</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>320152</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>355314</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CCC94DE-E74B-4545-9898-F89B8612FDBA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6843347" y="16771327"/>
+          <a:ext cx="276190" cy="333333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>323817</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>304768</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EEBB2C5-DA27-4E90-8FCC-1C18FBE84FF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858000" y="19850100"/>
+          <a:ext cx="266667" cy="257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>314292</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>323812</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Picture 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C9B2FBE-F0BF-4B23-95A9-7F337E0C6329}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6848475" y="20964525"/>
+          <a:ext cx="266667" cy="304762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>491773</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CF145AC-3903-4E2B-A314-76F5453750E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6858001" y="23260050"/>
+          <a:ext cx="434622" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>365791</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61EEC378-C978-4B4D-A1F5-8BD9E255FA13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6838950" y="22526625"/>
+          <a:ext cx="466725" cy="308641"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419057</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>304767</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE3D3AFC-F511-42ED-AD10-674238A4F09F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6877050" y="22126575"/>
+          <a:ext cx="342857" cy="266667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>331538</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6CE776A-8FDD-4F74-81BE-19649ADB0B18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6848475" y="22860001"/>
+          <a:ext cx="390525" cy="322012"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>373062</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C3FC5F3-1389-40AA-9876-357538D3B0FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6848475" y="21374100"/>
+          <a:ext cx="390525" cy="325437"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2401,9 +3073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1334683C-CBF3-44A7-AA05-85853A38880B}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2417,13 +3087,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>144</v>
+      <c r="A2" s="21" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2431,1088 +3101,1101 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="H5" s="15" t="s">
+      <c r="E5" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="16" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="42">
         <v>1</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="10"/>
+      <c r="D6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="11"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="40">
+      <c r="A8" s="45"/>
+      <c r="B8" s="33">
         <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="11"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="40"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="11"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="40"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="11"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="41">
+      <c r="A11" s="45"/>
+      <c r="B11" s="34">
         <v>3</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="11"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="11"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="46">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B13" s="42">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="11"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="43"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="11"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="44"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="39"/>
+      <c r="B16" s="33">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="11"/>
-    </row>
-    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="40">
-        <v>2</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="11"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="11"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="11"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="41">
+      <c r="A19" s="39"/>
+      <c r="B19" s="34">
         <v>3</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="20"/>
+      <c r="I19" s="19"/>
     </row>
     <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="41"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="20"/>
+      <c r="I20" s="19"/>
     </row>
     <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="41"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="34"/>
       <c r="C21" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="20"/>
+      <c r="I21" s="19"/>
     </row>
     <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="41"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="34"/>
       <c r="C22" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="20"/>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="41"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="34"/>
       <c r="C23" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="20"/>
+      <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
-      <c r="B24" s="41"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="34"/>
       <c r="C24" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="11"/>
+      <c r="I24" s="49"/>
     </row>
     <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="45">
+      <c r="A25" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="40">
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G25" s="3"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="11"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="36"/>
-      <c r="B26" s="45"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="40"/>
       <c r="C26" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G26" s="3"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="11"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="36"/>
-      <c r="B27" s="45"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G27" s="3"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="11"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
-      <c r="B28" s="45"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G28" s="3"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="11"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="36"/>
-      <c r="B29" s="45"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G29" s="3"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="11"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="36"/>
-      <c r="B30" s="40">
+      <c r="A30" s="41"/>
+      <c r="B30" s="33">
         <v>2</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="20"/>
+      <c r="I30" s="19"/>
     </row>
     <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
-      <c r="B31" s="40"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="33"/>
       <c r="C31" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="20"/>
+      <c r="I31" s="19"/>
     </row>
     <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
-      <c r="B32" s="40"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="33"/>
       <c r="C32" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="20"/>
+      <c r="I32" s="19"/>
     </row>
     <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
-      <c r="B33" s="40"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="20"/>
+      <c r="I33" s="19"/>
     </row>
     <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="36"/>
-      <c r="B34" s="40"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="33"/>
       <c r="C34" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="20"/>
+      <c r="I34" s="19"/>
     </row>
     <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="40">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="45">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="D35" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="11"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="37"/>
-      <c r="B36" s="45"/>
+      <c r="A36" s="35"/>
+      <c r="B36" s="40"/>
       <c r="C36" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="11"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="37"/>
-      <c r="B37" s="45"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="11"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="37"/>
-      <c r="B38" s="45"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="11"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="37"/>
-      <c r="B39" s="40">
+      <c r="A39" s="35"/>
+      <c r="B39" s="33">
         <v>2</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="11"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="37"/>
-      <c r="B40" s="40"/>
+      <c r="A40" s="35"/>
+      <c r="B40" s="33"/>
       <c r="C40" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="11"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="37"/>
-      <c r="B41" s="40"/>
+      <c r="A41" s="35"/>
+      <c r="B41" s="33"/>
       <c r="C41" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="11"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="37"/>
-      <c r="B42" s="41">
+      <c r="A42" s="35"/>
+      <c r="B42" s="34">
         <v>3</v>
       </c>
       <c r="C42" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G42" s="3"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="10"/>
+    </row>
+    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="35"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G42" s="3"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="11"/>
-    </row>
-    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="37"/>
-      <c r="B43" s="41"/>
-      <c r="C43" s="3" t="s">
+      <c r="E43" s="3"/>
+      <c r="F43" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="10"/>
+    </row>
+    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="35"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G43" s="3"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="11"/>
-    </row>
-    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="37"/>
-      <c r="B44" s="41"/>
-      <c r="C44" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="E44" s="3"/>
-      <c r="F44" s="3" t="s">
-        <v>139</v>
+      <c r="F44" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
-      <c r="I44" s="11"/>
+      <c r="I44" s="49"/>
     </row>
     <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="37"/>
+      <c r="A45" s="35"/>
       <c r="B45" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="D45" s="6" t="s">
         <v>104</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>105</v>
       </c>
       <c r="E45" s="6"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="11"/>
+      <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="24" t="s">
+      <c r="A46" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="23">
+        <v>1</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="46">
-        <v>1</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>98</v>
-      </c>
       <c r="D46" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E46" s="7"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-      <c r="I46" s="11"/>
+      <c r="I46" s="10"/>
     </row>
     <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="24"/>
-      <c r="B47" s="47" t="s">
-        <v>103</v>
+      <c r="A47" s="36"/>
+      <c r="B47" s="24" t="s">
+        <v>102</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E47" s="6"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
-      <c r="I47" s="11"/>
+      <c r="I47" s="10"/>
     </row>
     <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>117</v>
+      <c r="A48" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="37" t="s">
+        <v>116</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
-      <c r="I48" s="11"/>
+      <c r="I48" s="10"/>
     </row>
     <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
-      <c r="B49" s="8"/>
+      <c r="A49" s="38"/>
+      <c r="B49" s="37"/>
       <c r="C49" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
-      <c r="I49" s="11"/>
+      <c r="I49" s="10"/>
     </row>
     <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
-      <c r="B50" s="8"/>
+      <c r="A50" s="38"/>
+      <c r="B50" s="37"/>
       <c r="C50" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
-      <c r="I50" s="11"/>
+      <c r="I50" s="10"/>
     </row>
     <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="25"/>
-      <c r="B51" s="8" t="s">
-        <v>118</v>
+      <c r="A51" s="38"/>
+      <c r="B51" s="37" t="s">
+        <v>117</v>
       </c>
       <c r="C51" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>113</v>
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
-      <c r="I51" s="11"/>
+      <c r="I51" s="10"/>
     </row>
     <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="25"/>
-      <c r="B52" s="8"/>
+      <c r="A52" s="38"/>
+      <c r="B52" s="37"/>
       <c r="C52" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>115</v>
       </c>
       <c r="E52" s="6"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
-      <c r="I52" s="11"/>
+      <c r="I52" s="10"/>
     </row>
     <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
+      <c r="A53" s="38"/>
       <c r="B53" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
-      <c r="I53" s="11"/>
+      <c r="I53" s="10"/>
     </row>
     <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="21" t="s">
+      <c r="A54" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B54" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C54" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G54" s="18"/>
+      <c r="G54" s="17"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="11"/>
+      <c r="I54" s="10"/>
     </row>
     <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="22"/>
-      <c r="B55" s="29" t="s">
-        <v>15</v>
+      <c r="A55" s="31"/>
+      <c r="B55" s="26" t="s">
+        <v>14</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G55" s="17"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="10"/>
+    </row>
+    <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="31"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G55" s="18"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="11"/>
-    </row>
-    <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="22"/>
-      <c r="B56" s="29"/>
-      <c r="C56" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="D56" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G56" s="17"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="10"/>
+    </row>
+    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="31"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G56" s="18"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="11"/>
-    </row>
-    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="22"/>
-      <c r="B57" s="29"/>
-      <c r="C57" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="D57" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G57" s="17"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="10"/>
+    </row>
+    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="31"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G57" s="18"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="11"/>
-    </row>
-    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="22"/>
-      <c r="B58" s="29"/>
-      <c r="C58" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="D58" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G58" s="17"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="10"/>
+    </row>
+    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="31"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G58" s="18"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="11"/>
-    </row>
-    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="22"/>
-      <c r="B59" s="29"/>
-      <c r="C59" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="D59" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G59" s="18"/>
+        <v>51</v>
+      </c>
+      <c r="G59" s="17"/>
       <c r="H59" s="3"/>
-      <c r="I59" s="11"/>
+      <c r="I59" s="10"/>
     </row>
     <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
-      <c r="B60" s="30" t="s">
-        <v>30</v>
+      <c r="A60" s="31"/>
+      <c r="B60" s="27" t="s">
+        <v>29</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G60" s="18"/>
+        <v>70</v>
+      </c>
+      <c r="G60" s="17"/>
       <c r="H60" s="3"/>
-      <c r="I60" s="11"/>
+      <c r="I60" s="10"/>
     </row>
     <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="22"/>
-      <c r="B61" s="30"/>
+      <c r="A61" s="31"/>
+      <c r="B61" s="27"/>
       <c r="C61" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G61" s="18"/>
+        <v>64</v>
+      </c>
+      <c r="G61" s="17"/>
       <c r="H61" s="3"/>
-      <c r="I61" s="11"/>
+      <c r="I61" s="10"/>
     </row>
     <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="22"/>
-      <c r="B62" s="30"/>
+      <c r="A62" s="31"/>
+      <c r="B62" s="27"/>
       <c r="C62" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G62" s="17"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="10"/>
+    </row>
+    <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="31"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G62" s="18"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="11"/>
-    </row>
-    <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
-      <c r="B63" s="30"/>
-      <c r="C63" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="D63" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G63" s="18"/>
+        <v>68</v>
+      </c>
+      <c r="G63" s="17"/>
       <c r="H63" s="3"/>
-      <c r="I63" s="11"/>
+      <c r="I63" s="10"/>
     </row>
     <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="22"/>
-      <c r="B64" s="30"/>
+      <c r="A64" s="31"/>
+      <c r="B64" s="27"/>
       <c r="C64" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G64" s="18"/>
+        <v>69</v>
+      </c>
+      <c r="G64" s="17"/>
       <c r="H64" s="3"/>
-      <c r="I64" s="11"/>
+      <c r="I64" s="10"/>
     </row>
     <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="22"/>
-      <c r="B65" s="31" t="s">
-        <v>76</v>
+      <c r="A65" s="31"/>
+      <c r="B65" s="28" t="s">
+        <v>75</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G65" s="17"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="10"/>
+    </row>
+    <row r="66" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="32"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="G65" s="18"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="11"/>
-    </row>
-    <row r="66" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="23"/>
-      <c r="B66" s="32"/>
-      <c r="C66" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="G66" s="19"/>
-      <c r="H66" s="12"/>
-      <c r="I66" s="13"/>
+      <c r="D66" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E66" s="11"/>
+      <c r="F66" s="50" t="s">
+        <v>125</v>
+      </c>
+      <c r="G66" s="18"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:I66" xr:uid="{DAD6F9C2-C361-4C55-A71E-83FC06BFD5A2}"/>
   <mergeCells count="23">
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="A13:A24"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="A25:A34"/>
+    <mergeCell ref="B16:B18"/>
     <mergeCell ref="B55:B59"/>
     <mergeCell ref="B60:B64"/>
     <mergeCell ref="B65:B66"/>
@@ -3524,18 +4207,7 @@
     <mergeCell ref="B48:B50"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="A48:A53"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="A13:A24"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="A25:A34"/>
     <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" r:id="rId1"/>

</xml_diff>